<commit_message>
Change files for release 1.1.0 5584c4176ce6827e7acd2a06ebff3cc97513d77b
</commit_message>
<xml_diff>
--- a/feature/prepare-publication-1.0.1/ig/StructureDefinition-BundleAgregateur.xlsx
+++ b/feature/prepare-publication-1.0.1/ig/StructureDefinition-BundleAgregateur.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>1.1.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-04T08:15:55+00:00</t>
+    <t>2024-12-05T09:23:35+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>